<commit_message>
Sentence Label Sequence Completed
</commit_message>
<xml_diff>
--- a/Dataset Excel Sheets/ArabSign NumWords.xlsx
+++ b/Dataset Excel Sheets/ArabSign NumWords.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zaher.salman\Desktop\LINA JAN 24\Senior II\Senior-Design-Code\Dataset Excel Sheets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\salma\Desktop\Senior Design\CSE 491 - Senior Design II\github\Senior-Design-Code\Dataset Excel Sheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54952E9E-BCF6-42B7-8F1B-AB6F0B716F1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14380" windowHeight="4200" activeTab="1"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="166">
   <si>
     <t>SentenceID</t>
   </si>
@@ -393,12 +394,153 @@
   </si>
   <si>
     <t>50, 28, 30, 24</t>
+  </si>
+  <si>
+    <t>26, 64, 56, 34, 43</t>
+  </si>
+  <si>
+    <t>36, 10, 39, 44, 3</t>
+  </si>
+  <si>
+    <t>86, 55, 79, 13, 31</t>
+  </si>
+  <si>
+    <t>74, 36, 83, 71, 23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">41, 74, 62, </t>
+  </si>
+  <si>
+    <t>78, 59, 34</t>
+  </si>
+  <si>
+    <t>34, 11</t>
+  </si>
+  <si>
+    <t>78, 59, 62, 2</t>
+  </si>
+  <si>
+    <t>29, 34, 91</t>
+  </si>
+  <si>
+    <t>34, 73</t>
+  </si>
+  <si>
+    <t>34, 57</t>
+  </si>
+  <si>
+    <t>41, 74, 84</t>
+  </si>
+  <si>
+    <t>76, 70, 34</t>
+  </si>
+  <si>
+    <t>34, 67</t>
+  </si>
+  <si>
+    <t>34, 92, 50, 35</t>
+  </si>
+  <si>
+    <t>21, 53, 34</t>
+  </si>
+  <si>
+    <t>82, 50, 35</t>
+  </si>
+  <si>
+    <t>34, 53, 35, 63</t>
+  </si>
+  <si>
+    <t>60, 39</t>
+  </si>
+  <si>
+    <t>45, 39, 54</t>
+  </si>
+  <si>
+    <t>41, 48, 7, 15, 81</t>
+  </si>
+  <si>
+    <t>46, 79, 13, 85, 14</t>
+  </si>
+  <si>
+    <t>38, 51, 46, 79, 13</t>
+  </si>
+  <si>
+    <t>38, 58</t>
+  </si>
+  <si>
+    <t>42, 25</t>
+  </si>
+  <si>
+    <t>66, 1, 71, 37</t>
+  </si>
+  <si>
+    <t>18, 47, 85, 33</t>
+  </si>
+  <si>
+    <t>28, 48, 6, 50, 24</t>
+  </si>
+  <si>
+    <t>47, 85, 28, 49</t>
+  </si>
+  <si>
+    <t>47, 18, 85</t>
+  </si>
+  <si>
+    <t>90, 89</t>
+  </si>
+  <si>
+    <t>34, 80, 39</t>
+  </si>
+  <si>
+    <t>34, 72, 65</t>
+  </si>
+  <si>
+    <t>48, 34, 69</t>
+  </si>
+  <si>
+    <t>87, 39, 50</t>
+  </si>
+  <si>
+    <t>75, 40</t>
+  </si>
+  <si>
+    <t>34, 9</t>
+  </si>
+  <si>
+    <t>88, 61</t>
+  </si>
+  <si>
+    <t>86, 68, 77</t>
+  </si>
+  <si>
+    <t>17, 16</t>
+  </si>
+  <si>
+    <t>93, 32</t>
+  </si>
+  <si>
+    <t>27, 22</t>
+  </si>
+  <si>
+    <t>52, 19</t>
+  </si>
+  <si>
+    <t>80, 66, 5, 34</t>
+  </si>
+  <si>
+    <t>4, 39</t>
+  </si>
+  <si>
+    <t>34, 8</t>
+  </si>
+  <si>
+    <t>12, 79, 13</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -748,22 +890,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F51"/>
   <sheetViews>
     <sheetView zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
       <selection sqref="A1:B1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.1796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.54296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.54296875" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="97.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="97.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -774,7 +916,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -791,7 +933,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -806,7 +948,7 @@
       </c>
       <c r="F3" s="5"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
@@ -823,7 +965,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
@@ -838,7 +980,7 @@
       </c>
       <c r="F5" s="5"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
@@ -855,7 +997,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>12</v>
       </c>
@@ -870,7 +1012,7 @@
       </c>
       <c r="F7" s="5"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>14</v>
       </c>
@@ -887,7 +1029,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>16</v>
       </c>
@@ -902,7 +1044,7 @@
       </c>
       <c r="F9" s="5"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>18</v>
       </c>
@@ -919,7 +1061,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>20</v>
       </c>
@@ -934,7 +1076,7 @@
       </c>
       <c r="F11" s="5"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>22</v>
       </c>
@@ -952,7 +1094,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>24</v>
       </c>
@@ -967,7 +1109,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>26</v>
       </c>
@@ -978,7 +1120,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>28</v>
       </c>
@@ -989,7 +1131,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>30</v>
       </c>
@@ -1000,7 +1142,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>32</v>
       </c>
@@ -1011,7 +1153,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>34</v>
       </c>
@@ -1022,7 +1164,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>36</v>
       </c>
@@ -1033,7 +1175,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>38</v>
       </c>
@@ -1044,7 +1186,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>40</v>
       </c>
@@ -1055,7 +1197,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>42</v>
       </c>
@@ -1066,7 +1208,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>44</v>
       </c>
@@ -1077,7 +1219,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>46</v>
       </c>
@@ -1088,7 +1230,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>48</v>
       </c>
@@ -1099,7 +1241,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>50</v>
       </c>
@@ -1110,7 +1252,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>52</v>
       </c>
@@ -1121,7 +1263,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>54</v>
       </c>
@@ -1132,7 +1274,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>56</v>
       </c>
@@ -1143,7 +1285,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>58</v>
       </c>
@@ -1154,7 +1296,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>60</v>
       </c>
@@ -1165,7 +1307,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>62</v>
       </c>
@@ -1176,7 +1318,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>64</v>
       </c>
@@ -1187,7 +1329,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>66</v>
       </c>
@@ -1198,7 +1340,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>68</v>
       </c>
@@ -1209,7 +1351,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>70</v>
       </c>
@@ -1220,7 +1362,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>72</v>
       </c>
@@ -1231,7 +1373,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
         <v>74</v>
       </c>
@@ -1242,7 +1384,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
         <v>76</v>
       </c>
@@ -1253,7 +1395,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
         <v>78</v>
       </c>
@@ -1264,7 +1406,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
         <v>80</v>
       </c>
@@ -1275,7 +1417,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
         <v>82</v>
       </c>
@@ -1286,7 +1428,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
         <v>84</v>
       </c>
@@ -1297,7 +1439,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
         <v>86</v>
       </c>
@@ -1308,7 +1450,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
         <v>88</v>
       </c>
@@ -1319,7 +1461,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
         <v>90</v>
       </c>
@@ -1330,7 +1472,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
         <v>92</v>
       </c>
@@ -1341,7 +1483,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
         <v>94</v>
       </c>
@@ -1352,7 +1494,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
         <v>96</v>
       </c>
@@ -1363,7 +1505,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
         <v>98</v>
       </c>
@@ -1374,7 +1516,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
         <v>100</v>
       </c>
@@ -1393,21 +1535,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="C53" sqref="C53"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.1796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.54296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1418,7 +1560,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -1429,7 +1571,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -1440,7 +1582,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
@@ -1451,380 +1593,521 @@
         <v>118</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B5" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C5" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B6" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C6" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B7" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C7" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B8" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C8" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B9" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C9" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B10" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C10" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B11" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C11" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B12" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C12" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>24</v>
       </c>
       <c r="B13" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C13" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>26</v>
       </c>
       <c r="B14" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C14" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>28</v>
       </c>
       <c r="B15" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C15" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>30</v>
       </c>
       <c r="B16" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C16" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>32</v>
       </c>
       <c r="B17" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C17" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>34</v>
       </c>
       <c r="B18" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C18" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>36</v>
       </c>
       <c r="B19" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C19" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>38</v>
       </c>
       <c r="B20" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C20" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>40</v>
       </c>
       <c r="B21" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C21" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>42</v>
       </c>
       <c r="B22" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C22" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>44</v>
       </c>
       <c r="B23" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C23" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>46</v>
       </c>
       <c r="B24" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C24" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>48</v>
       </c>
       <c r="B25" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C25" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>50</v>
       </c>
       <c r="B26" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C26" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>52</v>
       </c>
       <c r="B27" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C27" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>54</v>
       </c>
       <c r="B28" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C28" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>56</v>
       </c>
       <c r="B29" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C29" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>58</v>
       </c>
       <c r="B30" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C30" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>60</v>
       </c>
       <c r="B31" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C31" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>62</v>
       </c>
       <c r="B32" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C32" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>64</v>
       </c>
       <c r="B33" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C33" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>66</v>
       </c>
       <c r="B34" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C34" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>68</v>
       </c>
       <c r="B35" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C35" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>70</v>
       </c>
       <c r="B36" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C36" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B37" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C37" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
         <v>74</v>
       </c>
       <c r="B38" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C38" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
         <v>76</v>
       </c>
       <c r="B39" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C39" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
         <v>78</v>
       </c>
       <c r="B40" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C40" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
         <v>80</v>
       </c>
       <c r="B41" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C41" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
         <v>82</v>
       </c>
       <c r="B42" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C42" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
         <v>84</v>
       </c>
       <c r="B43" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C43" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
         <v>86</v>
       </c>
       <c r="B44" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C44" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
         <v>88</v>
       </c>
       <c r="B45" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C45" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
         <v>90</v>
       </c>
       <c r="B46" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C46" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
         <v>92</v>
       </c>
       <c r="B47" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C47" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
         <v>94</v>
       </c>
       <c r="B48" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C48" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
         <v>96</v>
       </c>
       <c r="B49" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C49" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
         <v>98</v>
       </c>
       <c r="B50" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C50" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
         <v>100</v>
       </c>
       <c r="B51" t="s">
         <v>101</v>
+      </c>
+      <c r="C51" t="s">
+        <v>165</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
made resolution change MUCH faster
</commit_message>
<xml_diff>
--- a/Dataset Excel Sheets/ArabSign NumWords.xlsx
+++ b/Dataset Excel Sheets/ArabSign NumWords.xlsx
@@ -751,8 +751,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F51"/>
   <sheetViews>
-    <sheetView zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
-      <selection sqref="A1:B1048576"/>
+    <sheetView zoomScale="65" zoomScaleNormal="86" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1396,7 +1396,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="120" workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>

</xml_diff>